<commit_message>
Fixed battery and signal DSL issues
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_BatteryIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_BatteryIndicator_JS.xlsx
@@ -466,38 +466,6 @@
 validate1;
 link_Click(battery_test_link);
 validate2;
-SelectTestToRun(VT284_0012_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-TakeScreenshot(VT284_0012);
-validate4;
-</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT284-0012
-};
-validate4
-{
-validate_Screenshot=VT284_0012
-};</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(battery_test_link);
-validate2;
 SelectTestToRun(VT284_0015_string);
 ClickRunTest(runtest_top_xpath);
 validate3;
@@ -558,19 +526,6 @@
 };</t>
   </si>
   <si>
-    <t xml:space="preserve">wait(3);
-validate1;
-link_Click(battery_test_link);
-validate2;
-SelectTestToRun(VT284_0022_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(3);
-validate4;
-</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Manual specs
@@ -622,51 +577,73 @@
 };</t>
   </si>
   <si>
+    <t>stopbattery status without calling battery status</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT284-0003
+};
+validate4
+{
+validate_isIconDisplayed=batteryview_xpath,true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT284-0006
+};
+validate4
+{
+validate_isIconDisplayed=batteryview_xpath,true
+};</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT284-0012
+};
+validate4
+{
+validate_isIconDisplayed=batteryview_xpath,true
+};</t>
+  </si>
+  <si>
     <t>wait(3);
-PullConfigxml;
-ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
-ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
-ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="0"/&gt;);
-PushConfigxml;</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT284-0003
-};
-validate4
-{
-validate_Screenshot=VT284_0003
-};</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT284-0006
-};
-validate4
-{
-validate_Screenshot=VT284_0006
-};</t>
-  </si>
-  <si>
-    <t>stopbattery status without calling battery status</t>
+validate1;
+link_Click(battery_test_link);
+validate2;
+SelectTestToRun(VT284_0012_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+validate4;</t>
   </si>
   <si>
     <t xml:space="preserve">wait(3);
@@ -678,7 +655,6 @@
 validate3;
 ClickRunTest(runtest_bottom_xpath);
 wait(3);
-TakeScreenshot(VT284_0037);
 validate4;
 </t>
   </si>
@@ -697,8 +673,28 @@
 };
 validate4
 {
-validate_Screenshot=VT284_0037
+validate_isIconDisplayed=batteryview_xpath,false
 };</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(battery_test_link);
+validate2;
+SelectTestToRun(VT284_0022_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(3);
+validate4;</t>
+  </si>
+  <si>
+    <t>wait(3);
+PullConfigxml;
+ChangeConfigxml(Configuration/Applications/Application/General,StartPage,&lt;StartPage value="http://127.0.0.1:8082/app/" name="Menu"/&gt;);
+ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
+ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
+PushConfigxml;</t>
   </si>
 </sst>
 </file>
@@ -1163,7 +1159,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1229,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1525,7 +1523,7 @@
         <v>51</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -1552,7 +1550,7 @@
         <v>52</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1576,10 +1574,10 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -1603,10 +1601,10 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -1630,10 +1628,10 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -1657,10 +1655,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -1684,10 +1682,10 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -1705,16 +1703,16 @@
         <v>10</v>
       </c>
       <c r="E20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="F20" s="1">
-        <v>1</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H20" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>

</xml_diff>

<commit_message>
Adding emml and key handling modules to automation
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_BatteryIndicator_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/EBManual_BatteryIndicator_JS.xlsx
@@ -659,24 +659,6 @@
 </t>
   </si>
   <si>
-    <t>validate1
-{
-validate_PageTitle=Manual specs
-};
-validate2
-{
-validate_PageTitle=Battery JS Test
-};
-validate3
-{
-validate_Text_Exists=VT284-0037
-};
-validate4
-{
-validate_isIconDisplayed=batteryview_xpath,false
-};</t>
-  </si>
-  <si>
     <t>wait(3);
 validate1;
 link_Click(battery_test_link);
@@ -695,6 +677,24 @@
 ChangeConfigxml(Configuration,WebServer,&lt;WebServer&gt;endl  &lt;Enabled VALUE="1"/&gt;endl  &lt;Port VALUE="8082"/&gt;endl  &lt;WebFolder VALUE="\\auto\\manual_common_spec\"/&gt;endl  &lt;Public VALUE="1"/&gt;endl&lt;/WebServer&gt;endl);
 ChangeConfigxml(Configuration/Screen,FullScreen,&lt;FullScreen value="1"/&gt;);
 PushConfigxml;</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Manual specs
+};
+validate2
+{
+validate_PageTitle=Battery JS Test
+};
+validate3
+{
+validate_Text_Exists=VT284-0037
+};
+validate4
+{
+validate_Result=stopBatteryStatus : Called successfully
+};</t>
   </si>
 </sst>
 </file>
@@ -1160,7 +1160,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D3" sqref="D3:D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1227,7 +1227,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="2" t="s">
@@ -1655,7 +1655,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>57</v>
@@ -1691,7 +1691,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
     </row>
-    <row r="20" spans="1:11" ht="180.75" thickBot="1">
+    <row r="20" spans="1:11" ht="192" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>65</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>

</xml_diff>